<commit_message>
Adición de campo title
</commit_message>
<xml_diff>
--- a/sample/input.xlsx
+++ b/sample/input.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Documents\GitHub\concytec-pe\xlsx2skos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capacitacion\Documents\github\xlsx2skos\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E6E6D9-992F-4A03-8260-4F36B95666A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="renati_tipo" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>namespace</t>
   </si>
@@ -48,9 +47,6 @@
   </si>
   <si>
     <t>http://purl.org/pe-repo/renati/tipo</t>
-  </si>
-  <si>
-    <t>http://purl.org/pe-repo/renati/tipo/tesis</t>
   </si>
   <si>
     <t>Modalidad de obtención del grado
@@ -77,9 +73,6 @@
     <t>Tesis</t>
   </si>
   <si>
-    <t>http://purl.org/pe-repo/renati/tipo/trabajoDeInvestigacion</t>
-  </si>
-  <si>
     <t>Modalidad de
 obtención del grado académico que implica el proceso
 de generación de conocimiento en un determinado
@@ -97,9 +90,6 @@
   </si>
   <si>
     <t>Trabajo de investigación</t>
-  </si>
-  <si>
-    <t>http://purl.org/pe-repo/renati/tipo/trabajoDeSuficienciaProfesional</t>
   </si>
   <si>
     <t>Modalidad de titulación que implica que el bachiller está
@@ -125,9 +115,6 @@
     <t>Trabajo de suficiencia profesional</t>
   </si>
   <si>
-    <t>http://purl.org/pe-repo/renati/tipo/trabajoAcademico</t>
-  </si>
-  <si>
     <t>Modalidad de
 titulación que se desarrolla en el marco de un campo
 de estudio o área de conocimiento y que hace uso de,
@@ -145,11 +132,29 @@
   <si>
     <t>Trabajo académico</t>
   </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Tipos de trabajo de investigación (RENATI)</t>
+  </si>
+  <si>
+    <t>http://purl.org/pe-repo/renati/tipo#tesis</t>
+  </si>
+  <si>
+    <t>http://purl.org/pe-repo/renati/tipo#trabajoDeInvestigacion</t>
+  </si>
+  <si>
+    <t>http://purl.org/pe-repo/renati/tipo#trabajoDeSuficienciaProfesional</t>
+  </si>
+  <si>
+    <t>http://purl.org/pe-repo/renati/tipo#trabajoAcademico</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -222,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -238,9 +243,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,17 +558,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
@@ -573,87 +579,98 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
+      <c r="A5" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+      <c r="A6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>16</v>
+      <c r="A7" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" xr:uid="{58B9DE17-8E9B-47CC-A41E-7E7E45E4DE3B}"/>
+    <hyperlink ref="A8" r:id="rId1" location="trabajoAcademico"/>
+    <hyperlink ref="A5" r:id="rId2" location="tesis"/>
+    <hyperlink ref="A6" r:id="rId3" location="trabajoDeInvestigacion"/>
+    <hyperlink ref="A7" r:id="rId4" location="trabajoDeSuficienciaProfesional"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Plantilla y ejemplo de salida en html
</commit_message>
<xml_diff>
--- a/sample/input.xlsx
+++ b/sample/input.xlsx
@@ -26,12 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>namespace</t>
-  </si>
-  <si>
-    <t>uri</t>
   </si>
   <si>
     <t>definition_es</t>
@@ -136,26 +133,55 @@
     <t>title</t>
   </si>
   <si>
-    <t>Tipos de trabajo de investigación (RENATI)</t>
-  </si>
-  <si>
-    <t>http://purl.org/pe-repo/renati/tipo#tesis</t>
-  </si>
-  <si>
-    <t>http://purl.org/pe-repo/renati/tipo#trabajoDeInvestigacion</t>
-  </si>
-  <si>
-    <t>http://purl.org/pe-repo/renati/tipo#trabajoDeSuficienciaProfesional</t>
-  </si>
-  <si>
-    <t>http://purl.org/pe-repo/renati/tipo#trabajoAcademico</t>
+    <t>description</t>
+  </si>
+  <si>
+    <t>trabajoDeInvestigacion</t>
+  </si>
+  <si>
+    <t>tesis</t>
+  </si>
+  <si>
+    <t>preffix</t>
+  </si>
+  <si>
+    <t>trabajoDeSuficienciaProfesional</t>
+  </si>
+  <si>
+    <t>trabajoAcademico</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>Para efectos del presente Reglamento se utilizará
+el término “trabajo de investigación” para referirnos
+indistintamente a la tesis, al trabajo académico, al
+trabajo de sufciencia profesional y al propio trabajo de
+investigación en línea con lo señalado en el presente
+numeral. (Reglamento RENATI, RCD N° 033-2016-SUNEDU/CD, 4.15)</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>Concytec</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>0.1 (draft)</t>
+  </si>
+  <si>
+    <t>Vocabulario controlado para tipos de trabajo de investigación (RENATI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -164,23 +190,27 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -198,12 +228,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,11 +247,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -242,11 +265,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,10 +583,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -579,10 +600,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -590,87 +611,114 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f>CONCATENATE(B2, "#")</f>
+        <v>http://purl.org/pe-repo/renati/tipo#</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" location="trabajoAcademico"/>
-    <hyperlink ref="A5" r:id="rId2" location="tesis"/>
-    <hyperlink ref="A6" r:id="rId3" location="trabajoDeInvestigacion"/>
-    <hyperlink ref="A7" r:id="rId4" location="trabajoDeSuficienciaProfesional"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>